<commit_message>
class 33 & 32 codes, exceptions and write to excel
</commit_message>
<xml_diff>
--- a/testdata/Test.xlsx
+++ b/testdata/Test.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12768" windowHeight="9072"/>
+    <workbookView windowWidth="11520" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="TestSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="TestSheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -33,6 +34,9 @@
     <t>Zip</t>
   </si>
   <si>
+    <t>School</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
@@ -45,12 +49,21 @@
     <t>VA</t>
   </si>
   <si>
+    <t>syntax</t>
+  </si>
+  <si>
     <t>Jane</t>
   </si>
   <si>
     <t>New York</t>
   </si>
   <si>
+    <t>Fairfax</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -82,9 +95,6 @@
   </si>
   <si>
     <t>123 Holmes St</t>
-  </si>
-  <si>
-    <t>Fairfax</t>
   </si>
   <si>
     <t>pfeif11</t>
@@ -171,29 +181,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,20 +202,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -229,6 +210,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -237,16 +226,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,6 +249,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -277,30 +288,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,187 +325,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,6 +516,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -527,82 +611,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,148 +621,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1085,13 +1095,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
@@ -1112,40 +1122,68 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1"/>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>20151</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>12345</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>22304</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1172,19 +1210,19 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1196,118 +1234,118 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>7037777777</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>22030</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>8923949495</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>23040</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>7045938274</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4">
         <v>30495</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1335,4 +1373,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>